<commit_message>
Update CQL Execution Features spreadsheet based on recent work
</commit_message>
<xml_diff>
--- a/CQL_Execution_Features.xlsx
+++ b/CQL_Execution_Features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoesel/OneDrive - The MITRE Corporation/Documents/CDS_Connect/Task 2 Standards Conformance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoesel/dev/cqframework/cql-execution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473199ED-9000-4640-86F6-00BADA405570}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CEBA97-3660-5947-8BF1-B2E8511B2C65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16920" yWindow="460" windowWidth="34280" windowHeight="26720" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="820">
   <si>
     <t>Capability</t>
   </si>
@@ -2297,9 +2297,6 @@
     <t>* Implemented in logical.js (not nullological.js)</t>
   </si>
   <si>
-    <t>* Long not supported</t>
-  </si>
-  <si>
     <t>* Needs tests for standard use</t>
   </si>
   <si>
@@ -2309,41 +2306,13 @@
     <t>Arithmetic: MinValue</t>
   </si>
   <si>
-    <t>* Long not supported
-* Date/DateTime equality has new semantics
-* Needs tests for Decimal, String, Time, List, Interval, Null</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Needs tests for Date, DateTime, Time, Decimal, and Null</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Also needs tests for Date, Datetime, Time, Decimal, and Null</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Also needs tests for Date, DateTime, Time, Decimal, and Null</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Needs tests for Quantity and Null</t>
-  </si>
-  <si>
     <t>* Needs tests for Null</t>
   </si>
   <si>
-    <t>* Long not supported
-* Needs tests for Decimal, Quantity, Null, and Unrepresentable</t>
-  </si>
-  <si>
     <t>STU</t>
   </si>
   <si>
     <t>* Needs tests for Null and other precisions</t>
-  </si>
-  <si>
-    <t>* &amp; operator not supported</t>
   </si>
   <si>
     <t>* Implemented in comparison.js
@@ -2355,10 +2324,6 @@
 * Needs tests for Date and Time</t>
   </si>
   <si>
-    <t>* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
-* Needs tests for Date and Time</t>
-  </si>
-  <si>
     <t>* Implemented in comparison.js
 * Needs tests for Date and Time</t>
   </si>
@@ -2369,320 +2334,190 @@
     <t>* Needs tests for Date and Time</t>
   </si>
   <si>
-    <t>* Long not supported
-* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
+    <t>* Translated as SameOrAfter
+* Additional tests are probably not necessary</t>
+  </si>
+  <si>
+    <t>* Translated as SameOrBefore
+* Additional tests are probably not necessary</t>
+  </si>
+  <si>
+    <t>* Tests in comparison-tests.js
+* Needs tests for null (they're in CQL but not in the js)</t>
+  </si>
+  <si>
+    <t>* Translated as Not(Equivalent(a,b)) - so no extra implementation
+* Additional tests are probably not necessary</t>
+  </si>
+  <si>
+    <t>* Implementation supports Quantity type, but that's not in spec</t>
+  </si>
+  <si>
+    <t>* Needs tests for List with Null items (in test data but not in JS)</t>
+  </si>
+  <si>
+    <t>* Requires support from PatientSource</t>
+  </si>
+  <si>
+    <t>* Needs tests for List&lt;Code&gt;</t>
+  </si>
+  <si>
+    <t>* Boolean not supported</t>
+  </si>
+  <si>
+    <t>* Implemented in list.js</t>
+  </si>
+  <si>
+    <t>* Ratio not supported</t>
+  </si>
+  <si>
+    <t>* Needs tests for units other than years</t>
+  </si>
+  <si>
+    <t>* May require access to a terminology server</t>
+  </si>
+  <si>
+    <t>* Needs tests for Concept, List&lt;Concept&gt;, and List&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>* Implemented in nullological.js</t>
+  </si>
+  <si>
+    <t>* Implicitly tested in many tests</t>
+  </si>
+  <si>
+    <t>* Implicitly tested in many other tests</t>
+  </si>
+  <si>
+    <t>* Not supported as argument to function</t>
+  </si>
+  <si>
+    <t>* According to spec: Note that this operation should almost never be performed in practice. Code system references are allowed in order to allow for testing of code membership in a particular code system.</t>
+  </si>
+  <si>
+    <t>* Tested in instance-test.js</t>
+  </si>
+  <si>
+    <t>* CodeSystem property not supported</t>
+  </si>
+  <si>
+    <t>* Not supported w/ its own class, but extracted from Library</t>
+  </si>
+  <si>
+    <t>* Unclear if Practitioner context is actually part of the spec.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>* Retrieves not supported
+* References to expressions in other libraries not supported</t>
+  </si>
+  <si>
+    <t>* ParameterType property not supported (but may not be used)</t>
+  </si>
+  <si>
+    <t>External Data: Retrieve - contextProperty</t>
+  </si>
+  <si>
+    <t>Status Summary</t>
+  </si>
+  <si>
+    <t>GH Issue</t>
+  </si>
+  <si>
+    <t>156
+157</t>
+  </si>
+  <si>
+    <t>incorrect</t>
+  </si>
+  <si>
+    <t>199
+200</t>
+  </si>
+  <si>
+    <t>187
+201</t>
+  </si>
+  <si>
+    <t>202
+192</t>
+  </si>
+  <si>
+    <t>186
+177</t>
+  </si>
+  <si>
+    <t>* Needs tests for Quantity and Null</t>
+  </si>
+  <si>
+    <t>* Needs tests for null</t>
+  </si>
+  <si>
+    <t>* Semantics have changed for definite-duration vs calendar duration units
 * Needs tests for Date and Time</t>
   </si>
   <si>
-    <t>* Long not supported
-* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
-* Need to compare implementation to behavior defined in specification (it's complicated)
+    <t>* Needs tests for List with Null items</t>
+  </si>
+  <si>
+    <t>* Needs tests for Decimal, String, Time, List, Interval, Null</t>
+  </si>
+  <si>
+    <t>* Needs tests for Date, DateTime, Time, Decimal, and Null</t>
+  </si>
+  <si>
+    <t>* Needs tests for Decimal and Time</t>
+  </si>
+  <si>
+    <t>* Needs tests for Date, Datetime, Time, Decimal, and Null</t>
+  </si>
+  <si>
+    <t>* Needs tests for Date</t>
+  </si>
+  <si>
+    <t>* Needs tests for Decimal, Quantity, and Null</t>
+  </si>
+  <si>
+    <t>* Needs tests for Decimal, Quantity, Null, and Unrepresentable</t>
+  </si>
+  <si>
+    <t>* Some issues w/ very large numbers
+* Needs tests for Decimal and Null</t>
+  </si>
+  <si>
+    <t>* Whole number decimals may be treated like integers
+* Needs tests for Quantity, Date, Time, and Null</t>
+  </si>
+  <si>
+    <t>* Need to compare implementation to behavior defined in specification (it's complicated)
 * Needs tests for Date and Time</t>
   </si>
   <si>
-    <t>* Long not supported
-* Needs tests for Date and Time</t>
-  </si>
-  <si>
     <t>* Implemented in overloaded.js
-* Long not supported
 * Needs tests for Decimal, Date, and Time</t>
   </si>
   <si>
     <t>* Implemented in overloaded.js
 * Tests in comparison-tests.js
-* Long not supported
 * Needs tests for Decimal, Date, and Time</t>
   </si>
   <si>
-    <t>* Long not supported
-* Needs tests for Decimal, Quantity, Date, and Time</t>
-  </si>
-  <si>
-    <t>* Translated as SameOrAfter
-* Additional tests are probably not necessary</t>
-  </si>
-  <si>
-    <t>* Translated as SameOrBefore
-* Additional tests are probably not necessary</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
-* Needs tests for Quantity, Date, and Time</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
-* Needs tests for Decimal, Quantity, Date, and Time</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when list is null</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when list has multiple nulls</t>
-  </si>
-  <si>
-    <t>* Tests in comparison-tests.js
-* Needs tests for null (they're in CQL but not in the js)</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when second list is null</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Implementation incorrect when second list is null</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Implementation incorrect when first list is null</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when lists contain null</t>
-  </si>
-  <si>
-    <t>* Translated as Not(Equivalent(a,b)) - so no extra implementation
-* Additional tests are probably not necessary</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when list contains null</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when list is null
-* Needs test for when list is null</t>
-  </si>
-  <si>
-    <t>* Implementation supports Quantity type, but that's not in spec</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* String not supported</t>
-  </si>
-  <si>
-    <t>* Needs tests for List with Null items (in test data but not in JS)</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Tests are incomplete</t>
-  </si>
-  <si>
-    <t>* Requires support from PatientSource</t>
-  </si>
-  <si>
-    <t>* Long not supported
-* Needs tests for Decimal, Long, Integer</t>
-  </si>
-  <si>
-    <t>* Needs tests for List&lt;Code&gt;</t>
-  </si>
-  <si>
-    <t>* Boolean not supported</t>
-  </si>
-  <si>
-    <t>* Boolean and Long not supported</t>
-  </si>
-  <si>
-    <t>* Implemented in list.js</t>
-  </si>
-  <si>
-    <t>* Ratio not supported</t>
-  </si>
-  <si>
-    <t>* Needs tests for units other than years</t>
-  </si>
-  <si>
-    <t>* May require access to a terminology server</t>
-  </si>
-  <si>
-    <t>* Needs tests for Concept, List&lt;Concept&gt;, and List&lt;string&gt;</t>
-  </si>
-  <si>
-    <t>* Implemented in nullological.js</t>
-  </si>
-  <si>
-    <t>* Not all escape sequences seem to be supported</t>
-  </si>
-  <si>
-    <t>* Implicitly tested in many tests</t>
-  </si>
-  <si>
-    <t>* Implicitly tested in many other tests</t>
-  </si>
-  <si>
-    <t>* Not supported as argument to function</t>
-  </si>
-  <si>
-    <t>* According to spec: Note that this operation should almost never be performed in practice. Code system references are allowed in order to allow for testing of code membership in a particular code system.</t>
-  </si>
-  <si>
-    <t>* Tested in instance-test.js</t>
-  </si>
-  <si>
-    <t>* CodeSystem property not supported</t>
-  </si>
-  <si>
-    <t>* Not supported w/ its own class, but extracted from Library</t>
-  </si>
-  <si>
-    <t>* Unclear if Practitioner context is actually part of the spec.</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>* Retrieves not supported
-* References to expressions in other libraries not supported</t>
-  </si>
-  <si>
-    <t>* ParameterType property not supported (but may not be used)</t>
-  </si>
-  <si>
-    <t>External Data: Retrieve - contextProperty</t>
-  </si>
-  <si>
-    <t>Status Summary</t>
-  </si>
-  <si>
-    <t>* Implementation is incorrect (swapped with PopulationVariance)
-* Needs tests for List with Null items</t>
-  </si>
-  <si>
-    <t>GH Issue</t>
-  </si>
-  <si>
-    <t>156
-157</t>
-  </si>
-  <si>
-    <t>* Implementation is incorrect (swapped with StdDev)
-* Needs tests for List with Null items</t>
-  </si>
-  <si>
-    <t>* Implementation is incorrect (swapped with PopulationStdDev)
-* Needs tests for List with Null items</t>
-  </si>
-  <si>
-    <t>* Returns NaN for invalid operations (should be null)
-* Needs tests for Null</t>
-  </si>
-  <si>
-    <t>* Returns NaN for invalid operations (should be null)
-* Needs tests for null</t>
-  </si>
-  <si>
-    <t>* Returns NaN for invalid operations (should be null)
-* Long not supported
-* Needs tests for Decimal, Quantity, and Null</t>
-  </si>
-  <si>
-    <t>* Broken for (Quantity / Decimal)
-* Needs tests for Quantity and Null</t>
-  </si>
-  <si>
-    <t>* Implementaton for Decimal needs to be checked
-* Long not supported
-* Needs tests for Date</t>
-  </si>
-  <si>
-    <t>* Wrong answer for negative decimals
-* Needs tests for Null</t>
-  </si>
-  <si>
-    <t>* Wrong answer for negative decimals
-* Long not supported
-* Needs tests for Decimal, Quantity, and Null</t>
-  </si>
-  <si>
-    <t>incorrect</t>
-  </si>
-  <si>
-    <t>* Does not respect strict cast
-* Needs tests
-* Requires support from PatientSource</t>
-  </si>
-  <si>
-    <t>* Incorrect for some quantity checks
-* Long not supported
-* Date/DateTime equality has new semantics
-* Also needs tests for Decimal and Time</t>
+    <t>* Needs tests for Decimal, Quantity, Date, and Time</t>
   </si>
   <si>
     <t>* Not working correctly in test w/ "per 2 days"
-* Long not supported
 * Need to compare implementation to behavior defined in specification (it's complicated)</t>
   </si>
   <si>
-    <t>* Results in null when Interval is null (should be false)
-* Long not supported
-* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
-* Needs tests for Date and Time</t>
-  </si>
-  <si>
-    <t>* Incorrect w/ infinite intervals
-* Long not supported
-* Timezone normalization may currently be too aggressive (should only be normalized when precision is h/m/s/ms)
-* Needs tests for Date and Time</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect when list is null
-* Long not supported</t>
-  </si>
-  <si>
-    <t>* Should only return true if it matches entire input string</t>
-  </si>
-  <si>
-    <t>* Should return list of original string if separator is null</t>
-  </si>
-  <si>
-    <t>* Implementation incorrect for ToString(Time) when hours &lt; 10
-* Implementation incorrect for Time/DateTime when single-digit millis
-* Long not supported
-* Needs tests</t>
-  </si>
-  <si>
-    <t>199
-200</t>
-  </si>
-  <si>
-    <t>* Wrong answer for Power(null, null)
-* Some issues w/ very large numbers
-* Long not supported
-* Needs tests for Decimal and Null</t>
-  </si>
-  <si>
-    <t>187
-201</t>
-  </si>
-  <si>
-    <t>* Appears there may be issues w/ months between
-* Needs tests for Date and Time</t>
-  </si>
-  <si>
-    <t>202
-192</t>
-  </si>
-  <si>
-    <t>* Time should not have an offset</t>
-  </si>
-  <si>
-    <t>* Whole number decimals may be treated like integers
-* Long not supported
-* Needs tests for Quantity, Date, Time, and Null</t>
-  </si>
-  <si>
-    <t>* For quantities, may not use smallest unit in result (see GH issue)
-* Not supported for Uncertainties
-* Long not supported
-* Needs tests for Decimal, Quantity, and Null</t>
-  </si>
-  <si>
-    <t>* Not supported for Uncertainties
-* Long not supported
-* Needs tests for Quantity and Null</t>
-  </si>
-  <si>
-    <t>186
-177</t>
+    <t>* Needs tests for Quantity, Date, and Time</t>
+  </si>
+  <si>
+    <t>* Tests are incomplete</t>
+  </si>
+  <si>
+    <t>* Needs tests for Decimal, Long, Integer</t>
   </si>
 </sst>
 </file>
@@ -3210,7 +3045,7 @@
   <dimension ref="A1:J318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J96" sqref="J96"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3244,16 +3079,16 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>821</v>
+        <v>791</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>823</v>
+        <v>792</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3278,7 +3113,7 @@
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="8" t="s">
-        <v>810</v>
+        <v>780</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3305,7 +3140,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="8" t="s">
-        <v>807</v>
+        <v>778</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -3436,7 +3271,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -3450,18 +3285,16 @@
         <v>400</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="8" t="s">
-        <v>808</v>
-      </c>
+      <c r="I9" s="8"/>
       <c r="J9">
         <v>155</v>
       </c>
@@ -3641,7 +3474,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -3662,7 +3495,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -3682,10 +3515,10 @@
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="8" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>3.1</v>
       </c>
@@ -3708,10 +3541,10 @@
         <v>15</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>3.2</v>
       </c>
@@ -3736,7 +3569,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="8"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>3.3</v>
       </c>
@@ -3757,7 +3590,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="8"/>
     </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>4</v>
@@ -3778,10 +3611,10 @@
         <v>748</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>3.4</v>
       </c>
@@ -3806,7 +3639,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>3.5</v>
       </c>
@@ -3826,10 +3659,10 @@
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="8" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3.6</v>
       </c>
@@ -3852,10 +3685,10 @@
         <v>15</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>3.7</v>
       </c>
@@ -3880,7 +3713,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="8"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>3.8</v>
       </c>
@@ -3901,7 +3734,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>3.9</v>
       </c>
@@ -3924,10 +3757,10 @@
         <v>15</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -3950,7 +3783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>4</v>
@@ -3971,10 +3804,10 @@
         <v>748</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
@@ -3998,10 +3831,10 @@
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="8" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>37</v>
       </c>
@@ -4011,16 +3844,21 @@
         <v>421</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>14</v>
+        <v>748</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>14</v>
+        <v>748</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H32" s="6"/>
-      <c r="I32" s="8"/>
+      <c r="I32" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="J32">
+        <v>226</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
@@ -4063,7 +3901,7 @@
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="8" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4086,7 +3924,7 @@
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="8" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4109,7 +3947,7 @@
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="8" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4132,7 +3970,7 @@
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="8" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4155,7 +3993,7 @@
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="8" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -4207,7 +4045,7 @@
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="8" t="s">
-        <v>815</v>
+        <v>785</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4230,7 +4068,7 @@
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="8" t="s">
-        <v>815</v>
+        <v>785</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -4278,11 +4116,11 @@
         <v>15</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="8" t="s">
-        <v>816</v>
+        <v>786</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -4309,10 +4147,10 @@
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="8" t="s">
-        <v>818</v>
+        <v>788</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>824</v>
+        <v>793</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -4339,7 +4177,7 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="8" t="s">
-        <v>815</v>
+        <v>785</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4366,7 +4204,7 @@
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="8" t="s">
-        <v>819</v>
+        <v>789</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -4410,7 +4248,7 @@
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="8" t="s">
-        <v>809</v>
+        <v>779</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -5016,7 +4854,7 @@
         <v>15</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="8"/>
@@ -5083,7 +4921,7 @@
         <v>15</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="8"/>
@@ -5167,7 +5005,7 @@
         <v>15</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="8"/>
@@ -5204,7 +5042,7 @@
         <v>18</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>820</v>
+        <v>790</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>15</v>
@@ -5213,7 +5051,7 @@
         <v>15</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="8"/>
@@ -5297,7 +5135,7 @@
         <v>15</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="H86" s="6"/>
       <c r="I86" s="8"/>
@@ -5543,7 +5381,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>218</v>
       </c>
@@ -5557,7 +5395,7 @@
         <v>236</v>
       </c>
       <c r="E97" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F97" t="s">
         <v>748</v>
@@ -5566,10 +5404,10 @@
         <v>748</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>219</v>
       </c>
@@ -5583,7 +5421,7 @@
         <v>237</v>
       </c>
       <c r="E98" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F98" t="s">
         <v>748</v>
@@ -5592,13 +5430,13 @@
         <v>748</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
       <c r="J98">
         <v>190</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>220</v>
       </c>
@@ -5612,7 +5450,7 @@
         <v>238</v>
       </c>
       <c r="E99" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F99" t="s">
         <v>748</v>
@@ -5621,10 +5459,10 @@
         <v>748</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>221</v>
       </c>
@@ -5638,7 +5476,7 @@
         <v>578</v>
       </c>
       <c r="E100" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F100" t="s">
         <v>748</v>
@@ -5647,10 +5485,10 @@
         <v>748</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>222</v>
       </c>
@@ -5664,7 +5502,7 @@
         <v>239</v>
       </c>
       <c r="E101" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F101" t="s">
         <v>748</v>
@@ -5673,10 +5511,10 @@
         <v>748</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>223</v>
       </c>
@@ -5690,7 +5528,7 @@
         <v>579</v>
       </c>
       <c r="E102" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F102" t="s">
         <v>748</v>
@@ -5699,7 +5537,7 @@
         <v>748</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>760</v>
+        <v>804</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -5716,7 +5554,7 @@
         <v>580</v>
       </c>
       <c r="E103" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F103" t="s">
         <v>748</v>
@@ -5740,7 +5578,7 @@
         <v>240</v>
       </c>
       <c r="E104" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F104" t="s">
         <v>748</v>
@@ -6035,7 +5873,7 @@
       <c r="H116" s="6"/>
       <c r="I116" s="8"/>
     </row>
-    <row r="117" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>500</v>
       </c>
@@ -6049,7 +5887,7 @@
         <v>241</v>
       </c>
       <c r="E117" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F117" t="s">
         <v>748</v>
@@ -6058,10 +5896,10 @@
         <v>748</v>
       </c>
       <c r="I117" s="5" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>501</v>
       </c>
@@ -6075,7 +5913,7 @@
         <v>242</v>
       </c>
       <c r="E118" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F118" t="s">
         <v>748</v>
@@ -6084,7 +5922,7 @@
         <v>748</v>
       </c>
       <c r="I118" s="5" t="s">
-        <v>852</v>
+        <v>799</v>
       </c>
       <c r="J118">
         <v>177</v>
@@ -6113,10 +5951,10 @@
         <v>15</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>503</v>
       </c>
@@ -6130,7 +5968,7 @@
         <v>244</v>
       </c>
       <c r="E120" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F120" t="s">
         <v>748</v>
@@ -6139,7 +5977,7 @@
         <v>15</v>
       </c>
       <c r="I120" s="5" t="s">
-        <v>830</v>
+        <v>799</v>
       </c>
       <c r="J120">
         <v>183</v>
@@ -6168,7 +6006,7 @@
         <v>15</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -6194,7 +6032,7 @@
         <v>15</v>
       </c>
       <c r="I122" s="5" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
@@ -6223,7 +6061,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>507</v>
       </c>
@@ -6237,7 +6075,7 @@
         <v>248</v>
       </c>
       <c r="E124" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F124" t="s">
         <v>748</v>
@@ -6246,7 +6084,7 @@
         <v>15</v>
       </c>
       <c r="I124" s="5" t="s">
-        <v>827</v>
+        <v>756</v>
       </c>
       <c r="J124">
         <v>184</v>
@@ -6278,7 +6116,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>509</v>
       </c>
@@ -6292,7 +6130,7 @@
         <v>250</v>
       </c>
       <c r="E126" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F126" t="s">
         <v>748</v>
@@ -6301,13 +6139,13 @@
         <v>15</v>
       </c>
       <c r="I126" s="5" t="s">
-        <v>828</v>
+        <v>800</v>
       </c>
       <c r="J126">
         <v>184</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>510</v>
       </c>
@@ -6318,10 +6156,10 @@
         <v>101</v>
       </c>
       <c r="D127" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E127" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F127" t="s">
         <v>748</v>
@@ -6330,13 +6168,13 @@
         <v>748</v>
       </c>
       <c r="I127" s="5" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
       <c r="J127">
         <v>185</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>511</v>
       </c>
@@ -6347,10 +6185,10 @@
         <v>102</v>
       </c>
       <c r="D128" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E128" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F128" t="s">
         <v>748</v>
@@ -6359,13 +6197,13 @@
         <v>748</v>
       </c>
       <c r="I128" s="5" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
       <c r="J128">
         <v>185</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>512</v>
       </c>
@@ -6379,7 +6217,7 @@
         <v>251</v>
       </c>
       <c r="E129" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F129" t="s">
         <v>748</v>
@@ -6388,13 +6226,13 @@
         <v>748</v>
       </c>
       <c r="I129" s="5" t="s">
-        <v>829</v>
+        <v>808</v>
       </c>
       <c r="J129">
         <v>184</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>513</v>
       </c>
@@ -6408,7 +6246,7 @@
         <v>252</v>
       </c>
       <c r="E130" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F130" t="s">
         <v>748</v>
@@ -6417,13 +6255,13 @@
         <v>748</v>
       </c>
       <c r="I130" s="5" t="s">
-        <v>851</v>
+        <v>808</v>
       </c>
       <c r="J130" s="5" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>514</v>
       </c>
@@ -6437,7 +6275,7 @@
         <v>253</v>
       </c>
       <c r="E131" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F131" t="s">
         <v>748</v>
@@ -6446,10 +6284,10 @@
         <v>748</v>
       </c>
       <c r="I131" s="5" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>516</v>
       </c>
@@ -6463,7 +6301,7 @@
         <v>256</v>
       </c>
       <c r="E132" t="s">
-        <v>834</v>
+        <v>794</v>
       </c>
       <c r="F132" t="s">
         <v>748</v>
@@ -6472,10 +6310,10 @@
         <v>748</v>
       </c>
       <c r="I132" s="5" t="s">
-        <v>845</v>
+        <v>810</v>
       </c>
       <c r="J132" s="5" t="s">
-        <v>846</v>
+        <v>796</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
@@ -6504,7 +6342,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>517</v>
       </c>
@@ -6518,7 +6356,7 @@
         <v>255</v>
       </c>
       <c r="E134" t="s">
-        <v>834</v>
+        <v>794</v>
       </c>
       <c r="F134" t="s">
         <v>748</v>
@@ -6527,7 +6365,7 @@
         <v>748</v>
       </c>
       <c r="I134" s="5" t="s">
-        <v>850</v>
+        <v>811</v>
       </c>
       <c r="J134">
         <v>204</v>
@@ -6556,10 +6394,10 @@
         <v>15</v>
       </c>
       <c r="I135" s="5" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>519</v>
       </c>
@@ -6573,7 +6411,7 @@
         <v>258</v>
       </c>
       <c r="E136" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F136" t="s">
         <v>748</v>
@@ -6582,13 +6420,13 @@
         <v>748</v>
       </c>
       <c r="I136" s="5" t="s">
-        <v>852</v>
+        <v>799</v>
       </c>
       <c r="J136">
         <v>177</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>520</v>
       </c>
@@ -6602,7 +6440,7 @@
         <v>259</v>
       </c>
       <c r="E137" t="s">
-        <v>834</v>
+        <v>794</v>
       </c>
       <c r="F137" t="s">
         <v>748</v>
@@ -6611,13 +6449,13 @@
         <v>748</v>
       </c>
       <c r="I137" s="5" t="s">
-        <v>850</v>
+        <v>811</v>
       </c>
       <c r="J137">
         <v>204</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>521</v>
       </c>
@@ -6631,7 +6469,7 @@
         <v>260</v>
       </c>
       <c r="E138" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F138" t="s">
         <v>748</v>
@@ -6640,13 +6478,13 @@
         <v>15</v>
       </c>
       <c r="I138" s="5" t="s">
-        <v>832</v>
+        <v>756</v>
       </c>
       <c r="J138">
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>522</v>
       </c>
@@ -6660,7 +6498,7 @@
         <v>261</v>
       </c>
       <c r="E139" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F139" t="s">
         <v>748</v>
@@ -6669,7 +6507,7 @@
         <v>748</v>
       </c>
       <c r="I139" s="5" t="s">
-        <v>833</v>
+        <v>808</v>
       </c>
       <c r="J139">
         <v>189</v>
@@ -6698,7 +6536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>524</v>
       </c>
@@ -6712,16 +6550,13 @@
         <v>263</v>
       </c>
       <c r="E141" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F141" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G141" t="s">
         <v>15</v>
-      </c>
-      <c r="I141" s="5" t="s">
-        <v>766</v>
       </c>
       <c r="J141">
         <v>161</v>
@@ -6773,7 +6608,7 @@
         <v>15</v>
       </c>
       <c r="I143" s="5" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
     </row>
     <row r="144" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -6799,7 +6634,7 @@
         <v>15</v>
       </c>
       <c r="I144" s="5" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
@@ -6894,7 +6729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>534</v>
       </c>
@@ -6908,16 +6743,13 @@
         <v>269</v>
       </c>
       <c r="E149" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F149" t="s">
         <v>14</v>
       </c>
       <c r="G149" t="s">
         <v>15</v>
-      </c>
-      <c r="I149" s="5" t="s">
-        <v>841</v>
       </c>
       <c r="J149">
         <v>197</v>
@@ -6986,10 +6818,10 @@
         <v>271</v>
       </c>
       <c r="E152" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F152" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G152" t="s">
         <v>15</v>
@@ -6998,7 +6830,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>539</v>
       </c>
@@ -7012,16 +6844,13 @@
         <v>272</v>
       </c>
       <c r="E153" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F153" t="s">
         <v>14</v>
       </c>
       <c r="G153" t="s">
         <v>15</v>
-      </c>
-      <c r="I153" s="5" t="s">
-        <v>842</v>
       </c>
       <c r="J153">
         <v>198</v>
@@ -7119,7 +6948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>544</v>
       </c>
@@ -7133,7 +6962,7 @@
         <v>277</v>
       </c>
       <c r="E158" t="s">
-        <v>834</v>
+        <v>794</v>
       </c>
       <c r="F158" t="s">
         <v>748</v>
@@ -7142,13 +6971,13 @@
         <v>15</v>
       </c>
       <c r="I158" s="5" t="s">
-        <v>768</v>
+        <v>801</v>
       </c>
       <c r="J158">
         <v>191</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>554</v>
       </c>
@@ -7162,7 +6991,7 @@
         <v>278</v>
       </c>
       <c r="E159" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F159" t="s">
         <v>748</v>
@@ -7171,10 +7000,10 @@
         <v>15</v>
       </c>
       <c r="I159" s="5" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>555</v>
       </c>
@@ -7188,7 +7017,7 @@
         <v>279</v>
       </c>
       <c r="E160" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F160" t="s">
         <v>748</v>
@@ -7197,7 +7026,7 @@
         <v>15</v>
       </c>
       <c r="I160" s="5" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="161" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -7223,7 +7052,7 @@
         <v>15</v>
       </c>
       <c r="I161" s="5" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
     </row>
     <row r="162" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -7249,7 +7078,7 @@
         <v>15</v>
       </c>
       <c r="I162" s="5" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -7275,7 +7104,7 @@
         <v>15</v>
       </c>
       <c r="I163" s="5" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
@@ -7347,7 +7176,7 @@
         <v>15</v>
       </c>
       <c r="I166" s="5" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -7373,7 +7202,7 @@
         <v>15</v>
       </c>
       <c r="I167" s="5" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
     </row>
     <row r="168" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -7390,7 +7219,7 @@
         <v>550</v>
       </c>
       <c r="E168" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F168" t="s">
         <v>748</v>
@@ -7399,10 +7228,10 @@
         <v>15</v>
       </c>
       <c r="I168" s="5" t="s">
-        <v>847</v>
+        <v>763</v>
       </c>
       <c r="J168" s="5" t="s">
-        <v>848</v>
+        <v>797</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -7466,7 +7295,7 @@
         <v>283</v>
       </c>
       <c r="E171" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F171" t="s">
         <v>748</v>
@@ -7475,7 +7304,7 @@
         <v>15</v>
       </c>
       <c r="I171" s="5" t="s">
-        <v>779</v>
+        <v>764</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -7490,7 +7319,7 @@
         <v>284</v>
       </c>
       <c r="E172" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F172" t="s">
         <v>748</v>
@@ -7499,10 +7328,10 @@
         <v>15</v>
       </c>
       <c r="I172" s="5" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>566</v>
       </c>
@@ -7516,7 +7345,7 @@
         <v>575</v>
       </c>
       <c r="E173" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F173" t="s">
         <v>748</v>
@@ -7525,10 +7354,10 @@
         <v>15</v>
       </c>
       <c r="I173" s="5" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>567</v>
       </c>
@@ -7542,7 +7371,7 @@
         <v>576</v>
       </c>
       <c r="E174" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F174" t="s">
         <v>748</v>
@@ -7551,10 +7380,10 @@
         <v>15</v>
       </c>
       <c r="I174" s="5" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>568</v>
       </c>
@@ -7568,7 +7397,7 @@
         <v>577</v>
       </c>
       <c r="E175" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F175" t="s">
         <v>748</v>
@@ -7577,7 +7406,7 @@
         <v>15</v>
       </c>
       <c r="I175" s="5" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="68" x14ac:dyDescent="0.2">
@@ -7594,7 +7423,7 @@
         <v>285</v>
       </c>
       <c r="E176" t="s">
-        <v>834</v>
+        <v>794</v>
       </c>
       <c r="F176" t="s">
         <v>748</v>
@@ -7603,13 +7432,13 @@
         <v>15</v>
       </c>
       <c r="I176" s="5" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="J176">
         <v>191</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>570</v>
       </c>
@@ -7623,16 +7452,13 @@
         <v>286</v>
       </c>
       <c r="E177" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F177" t="s">
         <v>14</v>
       </c>
       <c r="G177" t="s">
         <v>15</v>
-      </c>
-      <c r="I177" s="5" t="s">
-        <v>849</v>
       </c>
       <c r="J177">
         <v>203</v>
@@ -7747,7 +7573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>590</v>
       </c>
@@ -7761,7 +7587,7 @@
         <v>289</v>
       </c>
       <c r="E183" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F183" t="s">
         <v>748</v>
@@ -7770,10 +7596,10 @@
         <v>748</v>
       </c>
       <c r="I183" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="184" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>591</v>
       </c>
@@ -7787,7 +7613,7 @@
         <v>290</v>
       </c>
       <c r="E184" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F184" t="s">
         <v>748</v>
@@ -7796,10 +7622,10 @@
         <v>748</v>
       </c>
       <c r="I184" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="185" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>592</v>
       </c>
@@ -7813,7 +7639,7 @@
         <v>291</v>
       </c>
       <c r="E185" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F185" t="s">
         <v>748</v>
@@ -7822,10 +7648,10 @@
         <v>748</v>
       </c>
       <c r="I185" s="5" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="186" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>593</v>
       </c>
@@ -7839,7 +7665,7 @@
         <v>292</v>
       </c>
       <c r="E186" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F186" t="s">
         <v>748</v>
@@ -7848,13 +7674,13 @@
         <v>748</v>
       </c>
       <c r="I186" s="5" t="s">
-        <v>838</v>
+        <v>763</v>
       </c>
       <c r="J186">
         <v>194</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>594</v>
       </c>
@@ -7868,7 +7694,7 @@
         <v>293</v>
       </c>
       <c r="E187" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F187" t="s">
         <v>748</v>
@@ -7877,10 +7703,10 @@
         <v>748</v>
       </c>
       <c r="I187" s="5" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>595</v>
       </c>
@@ -7894,7 +7720,7 @@
         <v>294</v>
       </c>
       <c r="E188" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F188" t="s">
         <v>748</v>
@@ -7903,10 +7729,10 @@
         <v>748</v>
       </c>
       <c r="I188" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>596</v>
       </c>
@@ -7920,7 +7746,7 @@
         <v>295</v>
       </c>
       <c r="E189" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F189" t="s">
         <v>748</v>
@@ -7929,10 +7755,10 @@
         <v>748</v>
       </c>
       <c r="I189" s="5" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="190" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>597</v>
       </c>
@@ -7946,7 +7772,7 @@
         <v>296</v>
       </c>
       <c r="E190" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F190" t="s">
         <v>748</v>
@@ -7955,10 +7781,10 @@
         <v>748</v>
       </c>
       <c r="I190" s="5" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="191" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>598</v>
       </c>
@@ -7972,7 +7798,7 @@
         <v>297</v>
       </c>
       <c r="E191" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F191" t="s">
         <v>748</v>
@@ -7981,10 +7807,10 @@
         <v>748</v>
       </c>
       <c r="I191" s="5" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>599</v>
       </c>
@@ -7998,7 +7824,7 @@
         <v>298</v>
       </c>
       <c r="E192" t="s">
-        <v>834</v>
+        <v>794</v>
       </c>
       <c r="F192" t="s">
         <v>748</v>
@@ -8007,13 +7833,13 @@
         <v>748</v>
       </c>
       <c r="I192" s="5" t="s">
-        <v>837</v>
+        <v>816</v>
       </c>
       <c r="J192">
         <v>193</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>600</v>
       </c>
@@ -8027,7 +7853,7 @@
         <v>299</v>
       </c>
       <c r="E193" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F193" t="s">
         <v>748</v>
@@ -8036,10 +7862,10 @@
         <v>748</v>
       </c>
       <c r="I193" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="194" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>601</v>
       </c>
@@ -8053,7 +7879,7 @@
         <v>300</v>
       </c>
       <c r="E194" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F194" t="s">
         <v>748</v>
@@ -8062,10 +7888,10 @@
         <v>748</v>
       </c>
       <c r="I194" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="195" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>602</v>
       </c>
@@ -8079,7 +7905,7 @@
         <v>583</v>
       </c>
       <c r="E195" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F195" t="s">
         <v>748</v>
@@ -8088,10 +7914,10 @@
         <v>748</v>
       </c>
       <c r="I195" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="196" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>603</v>
       </c>
@@ -8105,7 +7931,7 @@
         <v>301</v>
       </c>
       <c r="E196" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F196" t="s">
         <v>748</v>
@@ -8114,10 +7940,10 @@
         <v>748</v>
       </c>
       <c r="I196" s="5" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="197" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>604</v>
       </c>
@@ -8131,7 +7957,7 @@
         <v>302</v>
       </c>
       <c r="E197" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F197" t="s">
         <v>748</v>
@@ -8140,10 +7966,10 @@
         <v>748</v>
       </c>
       <c r="I197" s="5" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>605</v>
       </c>
@@ -8151,7 +7977,7 @@
         <v>585</v>
       </c>
       <c r="E198" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F198" t="s">
         <v>748</v>
@@ -8160,10 +7986,10 @@
         <v>748</v>
       </c>
       <c r="I198" s="5" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>606</v>
       </c>
@@ -8171,7 +7997,7 @@
         <v>584</v>
       </c>
       <c r="E199" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F199" t="s">
         <v>748</v>
@@ -8180,7 +8006,7 @@
         <v>748</v>
       </c>
       <c r="I199" s="5" t="s">
-        <v>778</v>
+        <v>815</v>
       </c>
     </row>
     <row r="200" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.2">
@@ -8221,7 +8047,7 @@
         <v>304</v>
       </c>
       <c r="E201" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F201" t="s">
         <v>748</v>
@@ -8245,7 +8071,7 @@
         <v>305</v>
       </c>
       <c r="E202" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F202" t="s">
         <v>748</v>
@@ -8254,7 +8080,7 @@
         <v>748</v>
       </c>
       <c r="I202" s="5" t="s">
-        <v>779</v>
+        <v>764</v>
       </c>
     </row>
     <row r="203" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -8269,7 +8095,7 @@
         <v>306</v>
       </c>
       <c r="E203" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F203" t="s">
         <v>748</v>
@@ -8278,10 +8104,10 @@
         <v>748</v>
       </c>
       <c r="I203" s="5" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="204" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>608</v>
       </c>
@@ -8295,7 +8121,7 @@
         <v>307</v>
       </c>
       <c r="E204" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F204" t="s">
         <v>748</v>
@@ -8304,10 +8130,10 @@
         <v>748</v>
       </c>
       <c r="I204" s="5" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>609</v>
       </c>
@@ -8315,7 +8141,7 @@
         <v>586</v>
       </c>
       <c r="E205" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F205" t="s">
         <v>748</v>
@@ -8324,10 +8150,10 @@
         <v>748</v>
       </c>
       <c r="I205" s="5" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="206" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>610</v>
       </c>
@@ -8335,7 +8161,7 @@
         <v>587</v>
       </c>
       <c r="E206" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F206" t="s">
         <v>748</v>
@@ -8344,7 +8170,7 @@
         <v>748</v>
       </c>
       <c r="I206" s="5" t="s">
-        <v>781</v>
+        <v>817</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
@@ -8419,7 +8245,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>614</v>
       </c>
@@ -8433,7 +8259,7 @@
         <v>309</v>
       </c>
       <c r="E210" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F210" t="s">
         <v>748</v>
@@ -8442,13 +8268,13 @@
         <v>748</v>
       </c>
       <c r="I210" s="5" t="s">
-        <v>839</v>
+        <v>763</v>
       </c>
       <c r="J210">
         <v>196</v>
       </c>
     </row>
-    <row r="211" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>615</v>
       </c>
@@ -8462,7 +8288,7 @@
         <v>310</v>
       </c>
       <c r="E211" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F211" t="s">
         <v>748</v>
@@ -8471,13 +8297,13 @@
         <v>748</v>
       </c>
       <c r="I211" s="5" t="s">
-        <v>839</v>
+        <v>763</v>
       </c>
       <c r="J211">
         <v>196</v>
       </c>
     </row>
-    <row r="212" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" t="s">
         <v>4</v>
@@ -8489,7 +8315,7 @@
         <v>311</v>
       </c>
       <c r="E212" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F212" t="s">
         <v>748</v>
@@ -8498,10 +8324,10 @@
         <v>748</v>
       </c>
       <c r="I212" s="5" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" t="s">
         <v>4</v>
@@ -8513,7 +8339,7 @@
         <v>312</v>
       </c>
       <c r="E213" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F213" t="s">
         <v>748</v>
@@ -8522,10 +8348,10 @@
         <v>748</v>
       </c>
       <c r="I213" s="5" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="214" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" t="s">
         <v>4</v>
@@ -8537,7 +8363,7 @@
         <v>313</v>
       </c>
       <c r="E214" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F214" t="s">
         <v>748</v>
@@ -8546,10 +8372,10 @@
         <v>748</v>
       </c>
       <c r="I214" s="5" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="215" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>616</v>
       </c>
@@ -8563,19 +8389,16 @@
         <v>314</v>
       </c>
       <c r="E215" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F215" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G215" t="s">
         <v>748</v>
       </c>
-      <c r="I215" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="216" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="216" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>617</v>
       </c>
@@ -8589,7 +8412,7 @@
         <v>315</v>
       </c>
       <c r="E216" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F216" t="s">
         <v>748</v>
@@ -8598,10 +8421,10 @@
         <v>748</v>
       </c>
       <c r="I216" s="5" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="217" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>618</v>
       </c>
@@ -8615,7 +8438,7 @@
         <v>316</v>
       </c>
       <c r="E217" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F217" t="s">
         <v>748</v>
@@ -8624,10 +8447,10 @@
         <v>748</v>
       </c>
       <c r="I217" s="5" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="218" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>619</v>
       </c>
@@ -8641,7 +8464,7 @@
         <v>317</v>
       </c>
       <c r="E218" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F218" t="s">
         <v>748</v>
@@ -8650,10 +8473,10 @@
         <v>748</v>
       </c>
       <c r="I218" s="5" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="219" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>620</v>
       </c>
@@ -8667,16 +8490,13 @@
         <v>318</v>
       </c>
       <c r="E219" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F219" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G219" t="s">
         <v>748</v>
-      </c>
-      <c r="I219" s="5" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
@@ -8696,7 +8516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>634</v>
       </c>
@@ -8710,16 +8530,13 @@
         <v>319</v>
       </c>
       <c r="E221" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F221" t="s">
         <v>14</v>
       </c>
       <c r="G221" t="s">
         <v>15</v>
-      </c>
-      <c r="I221" s="5" t="s">
-        <v>783</v>
       </c>
       <c r="J221">
         <v>164</v>
@@ -8742,7 +8559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>636</v>
       </c>
@@ -8756,16 +8573,13 @@
         <v>320</v>
       </c>
       <c r="E223" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F223" t="s">
         <v>14</v>
       </c>
       <c r="G223" t="s">
         <v>15</v>
-      </c>
-      <c r="I223" s="5" t="s">
-        <v>784</v>
       </c>
       <c r="J223">
         <v>165</v>
@@ -8808,7 +8622,7 @@
         <v>322</v>
       </c>
       <c r="E225" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F225" t="s">
         <v>748</v>
@@ -8817,10 +8631,10 @@
         <v>15</v>
       </c>
       <c r="I225" s="5" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="226" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>639</v>
       </c>
@@ -8834,16 +8648,13 @@
         <v>323</v>
       </c>
       <c r="E226" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F226" t="s">
         <v>14</v>
       </c>
       <c r="G226" t="s">
         <v>15</v>
-      </c>
-      <c r="I226" s="5" t="s">
-        <v>786</v>
       </c>
       <c r="J226">
         <v>166</v>
@@ -8952,7 +8763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>645</v>
       </c>
@@ -8966,22 +8777,19 @@
         <v>327</v>
       </c>
       <c r="E232" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F232" t="s">
         <v>14</v>
       </c>
       <c r="G232" t="s">
         <v>748</v>
-      </c>
-      <c r="I232" s="5" t="s">
-        <v>840</v>
       </c>
       <c r="J232">
         <v>164</v>
       </c>
     </row>
-    <row r="233" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>646</v>
       </c>
@@ -8995,7 +8803,7 @@
         <v>328</v>
       </c>
       <c r="E233" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F233" t="s">
         <v>14</v>
@@ -9003,11 +8811,8 @@
       <c r="G233" t="s">
         <v>748</v>
       </c>
-      <c r="I233" s="5" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="234" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>647</v>
       </c>
@@ -9021,16 +8826,13 @@
         <v>329</v>
       </c>
       <c r="E234" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F234" t="s">
         <v>14</v>
       </c>
       <c r="G234" t="s">
         <v>748</v>
-      </c>
-      <c r="I234" s="5" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.2">
@@ -9077,7 +8879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>649</v>
       </c>
@@ -9091,16 +8893,13 @@
         <v>332</v>
       </c>
       <c r="E237" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F237" t="s">
         <v>14</v>
       </c>
       <c r="G237" t="s">
         <v>15</v>
-      </c>
-      <c r="I237" s="5" t="s">
-        <v>789</v>
       </c>
       <c r="J237">
         <v>167</v>
@@ -9129,7 +8928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="B239" t="s">
         <v>4</v>
@@ -9141,16 +8940,13 @@
         <v>334</v>
       </c>
       <c r="E239" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F239" t="s">
         <v>14</v>
       </c>
       <c r="G239" t="s">
         <v>15</v>
-      </c>
-      <c r="I239" s="5" t="s">
-        <v>783</v>
       </c>
       <c r="J239">
         <v>168</v>
@@ -9203,7 +8999,7 @@
         <v>15</v>
       </c>
       <c r="I241" s="10" t="s">
-        <v>790</v>
+        <v>767</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.2">
@@ -9338,7 +9134,7 @@
         <v>338</v>
       </c>
       <c r="E248" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F248" t="s">
         <v>15</v>
@@ -9358,7 +9154,7 @@
         <v>630</v>
       </c>
       <c r="E249" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F249" t="s">
         <v>15</v>
@@ -9396,7 +9192,7 @@
         <v>339</v>
       </c>
       <c r="E251" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F251" t="s">
         <v>15</v>
@@ -9420,7 +9216,7 @@
         <v>340</v>
       </c>
       <c r="E252" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F252" t="s">
         <v>15</v>
@@ -9472,7 +9268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>664</v>
       </c>
@@ -9486,16 +9282,13 @@
         <v>342</v>
       </c>
       <c r="E255" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F255" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G255" t="s">
         <v>15</v>
-      </c>
-      <c r="I255" s="5" t="s">
-        <v>791</v>
       </c>
       <c r="J255">
         <v>172</v>
@@ -9547,7 +9340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
         <v>667</v>
       </c>
@@ -9561,16 +9354,13 @@
         <v>345</v>
       </c>
       <c r="E258" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F258" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G258" t="s">
         <v>15</v>
-      </c>
-      <c r="I258" s="5" t="s">
-        <v>792</v>
       </c>
       <c r="J258">
         <v>173</v>
@@ -9599,10 +9389,10 @@
         <v>15</v>
       </c>
       <c r="I259" s="5" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="260" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
         <v>669</v>
       </c>
@@ -9616,19 +9406,16 @@
         <v>351</v>
       </c>
       <c r="E260" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F260" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G260" t="s">
         <v>748</v>
       </c>
-      <c r="I260" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="261" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
         <v>670</v>
       </c>
@@ -9642,16 +9429,13 @@
         <v>347</v>
       </c>
       <c r="E261" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F261" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G261" t="s">
         <v>748</v>
-      </c>
-      <c r="I261" s="5" t="s">
-        <v>794</v>
       </c>
       <c r="J261">
         <v>181</v>
@@ -9680,10 +9464,10 @@
         <v>15</v>
       </c>
       <c r="I262" s="5" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="263" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>672</v>
       </c>
@@ -9697,22 +9481,19 @@
         <v>348</v>
       </c>
       <c r="E263" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F263" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G263" t="s">
         <v>748</v>
-      </c>
-      <c r="I263" s="5" t="s">
-        <v>794</v>
       </c>
       <c r="J263">
         <v>181</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
         <v>673</v>
       </c>
@@ -9726,19 +9507,16 @@
         <v>350</v>
       </c>
       <c r="E264" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F264" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G264" t="s">
         <v>748</v>
       </c>
-      <c r="I264" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="265" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="265" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>674</v>
       </c>
@@ -9752,7 +9530,7 @@
         <v>662</v>
       </c>
       <c r="E265" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F265" t="s">
         <v>748</v>
@@ -9761,13 +9539,13 @@
         <v>15</v>
       </c>
       <c r="I265" s="5" t="s">
-        <v>822</v>
+        <v>802</v>
       </c>
       <c r="J265">
         <v>49</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
         <v>675</v>
       </c>
@@ -9781,7 +9559,7 @@
         <v>663</v>
       </c>
       <c r="E266" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F266" t="s">
         <v>748</v>
@@ -9790,13 +9568,13 @@
         <v>15</v>
       </c>
       <c r="I266" s="5" t="s">
-        <v>825</v>
+        <v>802</v>
       </c>
       <c r="J266">
         <v>182</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
         <v>666</v>
       </c>
@@ -9810,19 +9588,16 @@
         <v>353</v>
       </c>
       <c r="E267" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F267" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G267" t="s">
         <v>748</v>
       </c>
-      <c r="I267" s="5" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="268" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="268" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>676</v>
       </c>
@@ -9836,7 +9611,7 @@
         <v>352</v>
       </c>
       <c r="E268" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F268" t="s">
         <v>748</v>
@@ -9845,13 +9620,13 @@
         <v>15</v>
       </c>
       <c r="I268" s="5" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
       <c r="J268">
         <v>182</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>677</v>
       </c>
@@ -9865,7 +9640,7 @@
         <v>354</v>
       </c>
       <c r="E269" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F269" t="s">
         <v>748</v>
@@ -9874,13 +9649,13 @@
         <v>15</v>
       </c>
       <c r="I269" s="5" t="s">
-        <v>822</v>
+        <v>802</v>
       </c>
       <c r="J269">
         <v>49</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
         <v>683</v>
       </c>
@@ -9894,7 +9669,7 @@
         <v>52</v>
       </c>
       <c r="E270" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F270" t="s">
         <v>15</v>
@@ -9903,7 +9678,7 @@
         <v>15</v>
       </c>
       <c r="I270" s="5" t="s">
-        <v>835</v>
+        <v>770</v>
       </c>
       <c r="J270">
         <v>174</v>
@@ -9972,7 +9747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>687</v>
       </c>
@@ -9986,7 +9761,7 @@
         <v>54</v>
       </c>
       <c r="E274" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F274" t="s">
         <v>748</v>
@@ -9995,7 +9770,7 @@
         <v>748</v>
       </c>
       <c r="I274" s="5" t="s">
-        <v>796</v>
+        <v>818</v>
       </c>
     </row>
     <row r="275" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -10021,7 +9796,7 @@
         <v>15</v>
       </c>
       <c r="I275" s="5" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.2">
@@ -10294,10 +10069,10 @@
         <v>15</v>
       </c>
       <c r="I287" s="5" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="288" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>701</v>
       </c>
@@ -10311,7 +10086,7 @@
         <v>68</v>
       </c>
       <c r="E288" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F288" t="s">
         <v>748</v>
@@ -10320,7 +10095,7 @@
         <v>748</v>
       </c>
       <c r="I288" s="5" t="s">
-        <v>798</v>
+        <v>819</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.2">
@@ -10363,7 +10138,7 @@
         <v>15</v>
       </c>
       <c r="I290" s="5" t="s">
-        <v>799</v>
+        <v>771</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.2">
@@ -10435,7 +10210,7 @@
         <v>15</v>
       </c>
       <c r="I293" s="5" t="s">
-        <v>800</v>
+        <v>772</v>
       </c>
     </row>
     <row r="294" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -10461,7 +10236,7 @@
         <v>748</v>
       </c>
       <c r="I294" s="5" t="s">
-        <v>801</v>
+        <v>772</v>
       </c>
     </row>
     <row r="295" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -10481,7 +10256,7 @@
         <v>15</v>
       </c>
       <c r="I295" s="5" t="s">
-        <v>802</v>
+        <v>773</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
@@ -10530,7 +10305,7 @@
         <v>15</v>
       </c>
       <c r="I297" s="5" t="s">
-        <v>803</v>
+        <v>774</v>
       </c>
       <c r="J297">
         <v>175</v>
@@ -10553,7 +10328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
         <v>712</v>
       </c>
@@ -10567,7 +10342,7 @@
         <v>76</v>
       </c>
       <c r="E299" t="s">
-        <v>834</v>
+        <v>14</v>
       </c>
       <c r="F299" t="s">
         <v>15</v>
@@ -10575,11 +10350,8 @@
       <c r="G299" t="s">
         <v>748</v>
       </c>
-      <c r="I299" s="5" t="s">
-        <v>843</v>
-      </c>
       <c r="J299" s="5" t="s">
-        <v>844</v>
+        <v>795</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.2">
@@ -10681,7 +10453,7 @@
         <v>15</v>
       </c>
       <c r="I304" s="5" t="s">
-        <v>804</v>
+        <v>775</v>
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.2">
@@ -10730,7 +10502,7 @@
         <v>15</v>
       </c>
       <c r="I306" s="5" t="s">
-        <v>804</v>
+        <v>775</v>
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.2">
@@ -10802,7 +10574,7 @@
         <v>15</v>
       </c>
       <c r="I309" s="5" t="s">
-        <v>805</v>
+        <v>776</v>
       </c>
     </row>
     <row r="310" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -10828,7 +10600,7 @@
         <v>15</v>
       </c>
       <c r="I310" s="5" t="s">
-        <v>806</v>
+        <v>777</v>
       </c>
     </row>
     <row r="311" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -10874,7 +10646,7 @@
       </c>
       <c r="H312" s="6"/>
       <c r="I312" s="8" t="s">
-        <v>805</v>
+        <v>776</v>
       </c>
     </row>
     <row r="313" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -10897,7 +10669,7 @@
       </c>
       <c r="H313" s="6"/>
       <c r="I313" s="8" t="s">
-        <v>805</v>
+        <v>776</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.2">
@@ -10980,10 +10752,10 @@
         <v>745</v>
       </c>
       <c r="E317" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F317" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G317" s="6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Fix interval expand function when unit is plural duration unit (#228)
* Fix interval expand function when unit is plural duration unit

Fixes #193

* Update features spreadsheet
</commit_message>
<xml_diff>
--- a/CQL_Execution_Features.xlsx
+++ b/CQL_Execution_Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoesel/dev/cqframework/cql-execution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CEBA97-3660-5947-8BF1-B2E8511B2C65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E92690-5D2B-6D46-984F-9777D283426E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16920" yWindow="460" windowWidth="34280" windowHeight="26720" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
   </bookViews>
@@ -2507,10 +2507,6 @@
     <t>* Needs tests for Decimal, Quantity, Date, and Time</t>
   </si>
   <si>
-    <t>* Not working correctly in test w/ "per 2 days"
-* Need to compare implementation to behavior defined in specification (it's complicated)</t>
-  </si>
-  <si>
     <t>* Needs tests for Quantity, Date, and Time</t>
   </si>
   <si>
@@ -2518,6 +2514,9 @@
   </si>
   <si>
     <t>* Needs tests for Decimal, Long, Integer</t>
+  </si>
+  <si>
+    <t>* Need to compare implementation to behavior defined in specification (it's complicated)</t>
   </si>
 </sst>
 </file>
@@ -7810,7 +7809,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>599</v>
       </c>
@@ -7824,7 +7823,7 @@
         <v>298</v>
       </c>
       <c r="E192" t="s">
-        <v>794</v>
+        <v>14</v>
       </c>
       <c r="F192" t="s">
         <v>748</v>
@@ -7833,7 +7832,7 @@
         <v>748</v>
       </c>
       <c r="I192" s="5" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
       <c r="J192">
         <v>193</v>
@@ -8130,7 +8129,7 @@
         <v>748</v>
       </c>
       <c r="I204" s="5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="205" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -8150,7 +8149,7 @@
         <v>748</v>
       </c>
       <c r="I205" s="5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="206" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -8170,7 +8169,7 @@
         <v>748</v>
       </c>
       <c r="I206" s="5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
@@ -9770,7 +9769,7 @@
         <v>748</v>
       </c>
       <c r="I274" s="5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="275" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -10095,7 +10094,7 @@
         <v>748</v>
       </c>
       <c r="I288" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implement support for user-provided MessageListener
Also provide a built-in NullMessageListener and ConsoleMessageListener.
</commit_message>
<xml_diff>
--- a/CQL_Execution_Features.xlsx
+++ b/CQL_Execution_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoesel/dev/cqframework/cql-execution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E92690-5D2B-6D46-984F-9777D283426E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B0954-28C4-D147-A11D-81CB66498049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="460" windowWidth="34280" windowHeight="26720" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
+    <workbookView xWindow="16920" yWindow="500" windowWidth="34280" windowHeight="26600" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
   </bookViews>
   <sheets>
     <sheet name="CQL 1.5" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="821">
   <si>
     <t>Capability</t>
   </si>
@@ -2517,6 +2517,9 @@
   </si>
   <si>
     <t>* Need to compare implementation to behavior defined in specification (it's complicated)</t>
+  </si>
+  <si>
+    <t>* Implemented for date-based types but not numeric types</t>
   </si>
 </sst>
 </file>
@@ -4444,13 +4447,13 @@
         <v>446</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="8"/>
@@ -4719,10 +4722,10 @@
         <v>458</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>14</v>
@@ -6315,7 +6318,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>515</v>
       </c>
@@ -6329,13 +6332,16 @@
         <v>254</v>
       </c>
       <c r="E133" t="s">
-        <v>15</v>
+        <v>748</v>
       </c>
       <c r="F133" t="s">
-        <v>15</v>
+        <v>748</v>
       </c>
       <c r="G133" t="s">
         <v>15</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>820</v>
       </c>
       <c r="J133">
         <v>160</v>
@@ -10685,10 +10691,10 @@
         <v>733</v>
       </c>
       <c r="E314" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F314" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G314" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Support for Message Operator (#247)
* Basic implementation of Message w/ console.log

* Implement support for user-provided MessageListener

Also provide a built-in NullMessageListener and ConsoleMessageListener.

* Fix typo
</commit_message>
<xml_diff>
--- a/CQL_Execution_Features.xlsx
+++ b/CQL_Execution_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoesel/dev/cqframework/cql-execution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E92690-5D2B-6D46-984F-9777D283426E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B0954-28C4-D147-A11D-81CB66498049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="460" windowWidth="34280" windowHeight="26720" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
+    <workbookView xWindow="16920" yWindow="500" windowWidth="34280" windowHeight="26600" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
   </bookViews>
   <sheets>
     <sheet name="CQL 1.5" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="821">
   <si>
     <t>Capability</t>
   </si>
@@ -2517,6 +2517,9 @@
   </si>
   <si>
     <t>* Need to compare implementation to behavior defined in specification (it's complicated)</t>
+  </si>
+  <si>
+    <t>* Implemented for date-based types but not numeric types</t>
   </si>
 </sst>
 </file>
@@ -4444,13 +4447,13 @@
         <v>446</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>748</v>
+        <v>14</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="8"/>
@@ -4719,10 +4722,10 @@
         <v>458</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>14</v>
@@ -6315,7 +6318,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>515</v>
       </c>
@@ -6329,13 +6332,16 @@
         <v>254</v>
       </c>
       <c r="E133" t="s">
-        <v>15</v>
+        <v>748</v>
       </c>
       <c r="F133" t="s">
-        <v>15</v>
+        <v>748</v>
       </c>
       <c r="G133" t="s">
         <v>15</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>820</v>
       </c>
       <c r="J133">
         <v>160</v>
@@ -10685,10 +10691,10 @@
         <v>733</v>
       </c>
       <c r="E314" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F314" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G314" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
maked implies operator as supported in excel sheet
</commit_message>
<xml_diff>
--- a/CQL_Execution_Features.xlsx
+++ b/CQL_Execution_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoesel/dev/cqframework/cql-execution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hossenlopp/code/abacus-repos/cql-execution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA126A1D-FE83-9D49-8AA0-224FA0B37764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3433B4-C2F5-E94A-B68D-D5664CC88ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56200" yWindow="1660" windowWidth="51200" windowHeight="26600" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
+    <workbookView xWindow="5920" yWindow="8680" windowWidth="34560" windowHeight="21580" xr2:uid="{BD7176B9-F4D7-4641-8174-C94C0FC4637E}"/>
   </bookViews>
   <sheets>
     <sheet name="CQL 1.5" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="836">
   <si>
     <t>Capability</t>
   </si>
@@ -2577,6 +2577,9 @@
   </si>
   <si>
     <t>294</t>
+  </si>
+  <si>
+    <t>158, 319</t>
   </si>
 </sst>
 </file>
@@ -2671,7 +2674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2697,11 +2700,40 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5F60"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -2762,34 +2794,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5F60"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2809,28 +2813,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFE3D192-473A-F64F-9B16-BDD036BAEF9D}" name="Table1" displayName="Table1" ref="A1:J318" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFE3D192-473A-F64F-9B16-BDD036BAEF9D}" name="Table1" displayName="Table1" ref="A1:J318" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:J318" xr:uid="{840FAC20-C910-0D4A-BC54-C8C26EB6B00E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{97C419BE-8AC9-CE46-BE00-F59ED57834C8}" name="Logical" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{97C419BE-8AC9-CE46-BE00-F59ED57834C8}" name="Logical" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{C88805A8-828E-6947-9F49-22481CDE564E}" name="Alt Page"/>
-    <tableColumn id="2" xr3:uid="{3C29D91D-3571-4E43-B6B8-0E58CA9D05E6}" name="Alt" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3C29D91D-3571-4E43-B6B8-0E58CA9D05E6}" name="Alt" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{77229700-2285-904F-B0CF-1C772D2DC797}" name="Capability"/>
     <tableColumn id="4" xr3:uid="{7259AA01-C65A-6D46-9E88-06C6BCEA2CD9}" name="Supported"/>
     <tableColumn id="5" xr3:uid="{84A190A3-FFAC-564D-8811-7377E5E613F1}" name="Tested"/>
     <tableColumn id="6" xr3:uid="{38CEE918-219A-4349-B3E9-41A70AF85329}" name="STU"/>
-    <tableColumn id="9" xr3:uid="{FE296567-86D1-6A48-824C-B5033A571F9A}" name="Status Summary" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{23CAA704-FC4C-1542-A57E-88E3323E03B8}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{73EEE41B-97DD-4F4B-80AB-7C5C7C415BC9}" name="GH Issue" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{FE296567-86D1-6A48-824C-B5033A571F9A}" name="Status Summary" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{23CAA704-FC4C-1542-A57E-88E3323E03B8}" name="Notes" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{73EEE41B-97DD-4F4B-80AB-7C5C7C415BC9}" name="GH Issue" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2868,7 +2872,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2974,7 +2978,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3116,7 +3120,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3126,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25183728-5293-364E-82DC-3D3D8A1E2D49}">
   <dimension ref="A1:J318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5837,16 +5841,16 @@
         <v>22</v>
       </c>
       <c r="E106" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F106" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G106" t="s">
         <v>15</v>
       </c>
-      <c r="J106" s="1">
-        <v>158</v>
+      <c r="J106" s="13" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
@@ -11202,17 +11206,17 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" dxfId="9" priority="4">
-      <formula>OR($E1="incorrect",AND($E1="no",$G1="no"))</formula>
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND($E1="no", $G1="yes")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND($E1="partial",$G1="partial")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>OR(AND($E1="partial",$G1="no"),AND($E1="no",$G1="partial"))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
-      <formula>AND($E1="partial",$G1="partial")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>AND($E1="no", $G1="yes")</formula>
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>OR($E1="incorrect",AND($E1="no",$G1="no"))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>